<commit_message>
3 neue Blätter hinzugefügt
</commit_message>
<xml_diff>
--- a/LPIC-1.xlsx
+++ b/LPIC-1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roman\Desktop\Neuer Ordner (2)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:2001_{CAE04CBB-E514-44E7-A8BF-D205CB49022C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:2001_{646488B5-D529-4635-8B59-91FA161663E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6000" yWindow="7545" windowWidth="43200" windowHeight="23535" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8850" yWindow="11565" windowWidth="29880" windowHeight="20775" firstSheet="6" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="03-15-Authentication" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,9 @@
     <sheet name="04-24 Dateien" sheetId="6" r:id="rId6"/>
     <sheet name="04-25 Head und Tail" sheetId="7" r:id="rId7"/>
     <sheet name="04-26 Less und more" sheetId="8" r:id="rId8"/>
+    <sheet name="04-27 Parameter nachschauen" sheetId="9" r:id="rId9"/>
+    <sheet name="04-28 Die Path-Variable" sheetId="10" r:id="rId10"/>
+    <sheet name="04-29 Programme Starten path" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="162913"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="145">
   <si>
     <t>Frage</t>
   </si>
@@ -390,6 +393,84 @@
   </si>
   <si>
     <t>tail -n 3 /var/log/boot.log</t>
+  </si>
+  <si>
+    <t>more spam1.txt</t>
+  </si>
+  <si>
+    <t>STRG + C</t>
+  </si>
+  <si>
+    <t>Du hast dich vertippt und möchtest deine Eingabe komplett löschen. (Uppercase)</t>
+  </si>
+  <si>
+    <t>Zeige die ersten paar Zeilen von spam1.txt an, mit der Möglichkeit (nur) nach unten mit ENTER durchzuscrollen.</t>
+  </si>
+  <si>
+    <t>Zeige die ersten paar Zeilen von spam1.txt an, mit der Möglichkeit mit Pfeiltasten nach unten + oben durchzuscrollen.</t>
+  </si>
+  <si>
+    <t>less spam1.txt</t>
+  </si>
+  <si>
+    <t>Wie beendest du das Programm less? (Uppercase)</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>head --help</t>
+  </si>
+  <si>
+    <t>Rufe die Hilfe zum Befehl "head" mit einem Parameter von "head" auf. Ausführlicher Parameter</t>
+  </si>
+  <si>
+    <t>head -n 4 text.txt</t>
+  </si>
+  <si>
+    <t>Aufruf von head mit 4 Zeilen (Kurzschreibweise) von datei text.txt.</t>
+  </si>
+  <si>
+    <t>Aufruf von head mit 4 Zeilen (Langschreibweise /Verbose) von datei text.txt.</t>
+  </si>
+  <si>
+    <t>head --lines=4 text.txt</t>
+  </si>
+  <si>
+    <t>Ausführliche Dokumentation zum Befehl head anzeigen lassen.</t>
+  </si>
+  <si>
+    <t>man head</t>
+  </si>
+  <si>
+    <t>Gib die Variable aus, die alle Pfade zu ausführbaren Befehlen (ohne Pfadangabe) beinhaltet.</t>
+  </si>
+  <si>
+    <t>echo $PATH</t>
+  </si>
+  <si>
+    <t>Gib den Pfad aus, von dem aus der Befehl cat gestartet wird.</t>
+  </si>
+  <si>
+    <t>which cat</t>
+  </si>
+  <si>
+    <t>Ich möchte eine Datei ausführen können. Was sollte ich Ganz oben in die Datei schreiben, wenn die Datei mit bash laufen soll?</t>
+  </si>
+  <si>
+    <t>#!/bin/bash</t>
+  </si>
+  <si>
+    <t>export PATH=$PATH:~/bin</t>
+  </si>
+  <si>
+    <t>:</t>
+  </si>
+  <si>
+    <t>Was trennt einzelne Pfade in der PATH-Variable voneinander?</t>
+  </si>
+  <si>
+    <t>Setze die Variable PATH auf den bisherigen Inhalt und füge ~/bin hinzu (erstmal nur temporär)</t>
   </si>
 </sst>
 </file>
@@ -836,6 +917,99 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4B9A7C3-8117-47F3-BDAE-823BC11FD3F1}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="84.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F84BDF7D-DEC1-439E-B1D8-5715028080F7}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="115.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA0BD566-F0A2-4751-8B1A-8396B15F53DE}">
   <dimension ref="A1:B13"/>
@@ -1368,12 +1542,118 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F02DE26-447E-49D4-84A4-A31462C006D2}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="91.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE157A2E-ED0B-44EC-BA1B-83850810F5CB}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="87.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Mit Enrico gemacht auf blatt
</commit_message>
<xml_diff>
--- a/LPIC-1.xlsx
+++ b/LPIC-1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roman\Desktop\Neuer Ordner (2)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sysadmin\lernplattform_5.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:2001_{646488B5-D529-4635-8B59-91FA161663E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{153CF4F2-54A3-4424-96C6-5AEE36111B92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8850" yWindow="11565" windowWidth="29880" windowHeight="20775" firstSheet="6" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="10" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="03-15-Authentication" sheetId="1" r:id="rId1"/>
@@ -24,9 +24,11 @@
     <sheet name="04-27 Parameter nachschauen" sheetId="9" r:id="rId9"/>
     <sheet name="04-28 Die Path-Variable" sheetId="10" r:id="rId10"/>
     <sheet name="04-29 Programme Starten path" sheetId="11" r:id="rId11"/>
+    <sheet name="05-36 Pakete über das Terminal" sheetId="12" r:id="rId12"/>
+    <sheet name="05-37 Pakete + Quellen suchen" sheetId="13" r:id="rId13"/>
+    <sheet name="05-38 Skype nachinstallieren" sheetId="14" r:id="rId14"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="167">
   <si>
     <t>Frage</t>
   </si>
@@ -471,6 +473,72 @@
   </si>
   <si>
     <t>Setze die Variable PATH auf den bisherigen Inhalt und füge ~/bin hinzu (erstmal nur temporär)</t>
+  </si>
+  <si>
+    <t>UBUNTU: Update die Paketlisten</t>
+  </si>
+  <si>
+    <t>apt update</t>
+  </si>
+  <si>
+    <t>apt upgrade</t>
+  </si>
+  <si>
+    <t>apt dist-upgrade</t>
+  </si>
+  <si>
+    <t>Aktualisiere und installiere die neueste Version aller Pakete ohne neue Abhängigkeiten</t>
+  </si>
+  <si>
+    <t>Aktualisiere und installiere die neueste Version aller Pakete mit neuen Abhängigkeiten</t>
+  </si>
+  <si>
+    <t>UBUNTU: Installiere htop</t>
+  </si>
+  <si>
+    <t>apt install htop</t>
+  </si>
+  <si>
+    <t>apt-get install php</t>
+  </si>
+  <si>
+    <t>Alternativer Debianbefehl (nicht apt, nicht apt-get) um php zu installieren</t>
+  </si>
+  <si>
+    <t>Alternativer Debianbefehl (nicht apt, nicht aptitude) um php zu installieren</t>
+  </si>
+  <si>
+    <t>aptitude install php</t>
+  </si>
+  <si>
+    <t>Suche in den Paketlisten nach php</t>
+  </si>
+  <si>
+    <t>apt search php</t>
+  </si>
+  <si>
+    <t>Website für Ubuntu packages</t>
+  </si>
+  <si>
+    <t>packages.ubuntu.com</t>
+  </si>
+  <si>
+    <t>Website für Debian packages</t>
+  </si>
+  <si>
+    <t>packages.debian.org</t>
+  </si>
+  <si>
+    <t>Wo liegen die Konfigurationsdatein für den Paketmanager apt?</t>
+  </si>
+  <si>
+    <t>/etc/apt/sources.list</t>
+  </si>
+  <si>
+    <t>Wo liegen die Konfigurationsdateien für selbst installierte Pakete mit dpkg?</t>
+  </si>
+  <si>
+    <t>/etc/apt/sources.list.d/</t>
   </si>
 </sst>
 </file>
@@ -963,7 +1031,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F84BDF7D-DEC1-439E-B1D8-5715028080F7}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -1003,6 +1071,171 @@
       </c>
       <c r="B4" t="s">
         <v>142</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C09F1CAF-F311-46EC-A20E-CE34CCDEF86D}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="80.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>150</v>
+      </c>
+      <c r="B4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B592CA16-AC89-4F72-9B54-2C34E7D7D473}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="69" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>157</v>
+      </c>
+      <c r="B4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>159</v>
+      </c>
+      <c r="B5" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>161</v>
+      </c>
+      <c r="B6" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>163</v>
+      </c>
+      <c r="B7" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>165</v>
+      </c>
+      <c r="B8" t="s">
+        <v>166</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BCA7220-F963-44E1-B0D1-4EB93011CB89}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>